<commit_message>
add almost final version
</commit_message>
<xml_diff>
--- a/measures.xlsx
+++ b/measures.xlsx
@@ -445,24 +445,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="124026240"/>
-        <c:axId val="124044800"/>
+        <c:axId val="119673984"/>
+        <c:axId val="119675520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="124026240"/>
+        <c:axId val="119673984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124044800"/>
+        <c:crossAx val="119675520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124044800"/>
+        <c:axId val="119675520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,7 +470,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124026240"/>
+        <c:crossAx val="119673984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -483,7 +483,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -794,24 +794,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="129296256"/>
-        <c:axId val="129297792"/>
+        <c:axId val="119726464"/>
+        <c:axId val="119728000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129296256"/>
+        <c:axId val="119726464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129297792"/>
+        <c:crossAx val="119728000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129297792"/>
+        <c:axId val="119728000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +819,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129296256"/>
+        <c:crossAx val="119726464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -832,7 +832,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1075,25 +1075,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="127224064"/>
-        <c:axId val="129294720"/>
+        <c:axId val="62619008"/>
+        <c:axId val="62624896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127224064"/>
+        <c:axId val="62619008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129294720"/>
+        <c:crossAx val="62624896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129294720"/>
+        <c:axId val="62624896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1101,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127224064"/>
+        <c:crossAx val="62619008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1114,7 +1114,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1193,25 +1193,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126527744"/>
-        <c:axId val="127201280"/>
+        <c:axId val="62648704"/>
+        <c:axId val="62650240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126527744"/>
+        <c:axId val="62648704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127201280"/>
+        <c:crossAx val="62650240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127201280"/>
+        <c:axId val="62650240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1219,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126527744"/>
+        <c:crossAx val="62648704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1232,7 +1232,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>